<commit_message>
convert additional SBML ODE test suite models to wc lang, with rate laws using species concentration converted to use species population; work on debugging ODE submodel and models that don't properly solve; calculate the derivatives of species from expected population trajectories; play with 2 SSA submodels
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/semantic/00001/00001-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/semantic/00001/00001-wc_lang.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
-  <workbookPr/>
+  <workbookPr showObjects="placeholders"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/semantic/00001/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-24000" yWindow="2760" windowWidth="23980" windowHeight="9800" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="7160" windowWidth="34180" windowHeight="5060" tabRatio="500" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4228,7 +4228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="199">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 16:22:38'</t>
   </si>
@@ -4692,9 +4692,6 @@
     <t>!Intention type</t>
   </si>
   <si>
-    <t>test_case_00001</t>
-  </si>
-  <si>
     <t>ode_submodel</t>
   </si>
   <si>
@@ -4722,9 +4719,6 @@
     <t>normal_distribution</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>density_c</t>
   </si>
   <si>
@@ -4764,9 +4758,6 @@
     <t>forward</t>
   </si>
   <si>
-    <t>k1 * S1[c]</t>
-  </si>
-  <si>
     <t>k1</t>
   </si>
   <si>
@@ -4788,9 +4779,6 @@
     <t>dist-init-conc-S2[c]</t>
   </si>
   <si>
-    <t>1 / (molecule * second)</t>
-  </si>
-  <si>
     <t>s^-1</t>
   </si>
   <si>
@@ -4800,20 +4788,54 @@
     <t>gram / liter</t>
   </si>
   <si>
-    <t>density not used</t>
-  </si>
-  <si>
     <t>Basic single forward reaction with two species in one compartment</t>
+  </si>
+  <si>
+    <t>Density compartment c</t>
+  </si>
+  <si>
+    <t>Avogadro</t>
+  </si>
+  <si>
+    <t>molecule / mole</t>
+  </si>
+  <si>
+    <t>c1_units</t>
+  </si>
+  <si>
+    <t>Units factor for conv_1 function for rate law 1</t>
+  </si>
+  <si>
+    <t>1 / (molecule liter)</t>
+  </si>
+  <si>
+    <t>vol_c</t>
+  </si>
+  <si>
+    <t>Volume of compartment c</t>
+  </si>
+  <si>
+    <t>c / density_c</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>test_case_00001_converted</t>
+  </si>
+  <si>
+    <t>c1_units * k1 * S1[c] * c / density_c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4851,6 +4873,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4920,7 +4956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4942,9 +4978,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4972,35 +5005,63 @@
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5305,10 +5366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5593,10 +5651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5787,14 +5842,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5841,10 +5899,18 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>196</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -5928,47 +5994,27 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:I2"/>
   <dataValidations count="9">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A12">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A10">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B10">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C3:C12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D3:D12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E3:E12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F3:F12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G3:G12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H3:H12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C3:C10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D3:D10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E3:E10"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F3:F10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G3:G10"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H3:H10">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I3:I12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I3:I10"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5979,10 +6025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6015,13 +6058,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="36" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6075,23 +6118,23 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>175</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6308,14 +6351,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="8" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6374,21 +6421,22 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="A3" s="3" t="s">
         <v>177</v>
       </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>187</v>
+      <c r="F3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6480,78 +6528,35 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:L2"/>
-  <dataValidations count="12">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A12">
+  <dataValidations count="11">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B9">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D4:D12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A9">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D3:D9">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E3:E12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E3:E9">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F4:F12"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G3:G12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F3:F9"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G3:G9">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H9"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I9"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J9"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K9">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L12"/>
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="C3">
-      <formula1>1</formula1>
-      <formula2>63</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B4:B12 D3">
-      <formula1>255</formula1>
-    </dataValidation>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L9"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6562,7 +6567,7 @@
           <x14:formula1>
             <xm:f>'!!Reactions'!$A$4:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C12 F3</xm:sqref>
+          <xm:sqref>C3:C9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6574,10 +6579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6827,10 +6829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7049,10 +7048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7291,16 +7287,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="11" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -7311,8 +7309,8 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -7321,22 +7319,22 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="21" t="s">
         <v>76</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="21" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -7356,15 +7354,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="D3" s="25">
+      <c r="A3" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="30">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>186</v>
+      <c r="E3" s="28">
+        <v>0</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>174</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -7374,34 +7376,42 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="26">
+      <c r="D4" s="20">
         <v>1</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>189</v>
+      <c r="F4" s="26" t="s">
+        <v>185</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="32">
+        <v>6.0221408570000002E+23</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>189</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -7409,12 +7419,22 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>191</v>
+      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="20">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>192</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -7423,11 +7443,11 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -7438,9 +7458,9 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -7451,9 +7471,9 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -7464,8 +7484,8 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -7477,8 +7497,8 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -7490,8 +7510,8 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -7524,7 +7544,7 @@
       <formula1>4294967295</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K3:K12"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E4:E12 D3">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="D3 E4:E12">
       <formula1>-1E-100</formula1>
     </dataValidation>
   </dataValidations>
@@ -7537,10 +7557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7731,10 +7748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7776,42 +7790,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="36" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="S2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="36" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8224,12 +8238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="B3:D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8259,7 +8268,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8277,7 +8286,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -8505,10 +8514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8652,10 +8658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8688,10 +8691,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="36" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -8955,10 +8958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9310,10 +9310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9566,10 +9563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9907,12 +9901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9942,7 +9931,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9974,7 +9963,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10006,7 +9995,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10057,12 +10046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10219,10 +10203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10270,13 +10251,13 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="3"/>
@@ -10402,14 +10383,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.6640625" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="21" width="15.6640625" customWidth="1"/>
     <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10446,29 +10427,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="36" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="36" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10542,38 +10523,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:21" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>161</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="I4" s="37">
         <v>1</v>
       </c>
       <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>165</v>
+      <c r="K4" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -10593,8 +10574,8 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -10864,10 +10845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10896,22 +10874,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="36" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -10967,10 +10945,10 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10982,23 +10960,23 @@
       <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>169</v>
+      <c r="I4" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="14" t="s">
-        <v>168</v>
+      <c r="M4" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -11010,14 +10988,14 @@
       <c r="H5" s="3">
         <v>0</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>169</v>
+      <c r="I5" s="13" t="s">
+        <v>167</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="14" t="s">
-        <v>168</v>
+      <c r="M5" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -11197,10 +11175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E4"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11255,18 +11230,18 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>170</v>
+      <c r="A3" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11275,18 +11250,18 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>171</v>
+      <c r="A4" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -11437,10 +11412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11504,23 +11476,23 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="D3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="18">
-        <v>1.4999999999999999E-4</v>
-      </c>
-      <c r="F3" s="16">
-        <v>0</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>172</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -11530,23 +11502,23 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="15" t="s">
-        <v>171</v>
+      <c r="C4" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" s="15">
+        <v>162</v>
+      </c>
+      <c r="E4" s="14">
         <v>0</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <v>0</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>172</v>
+      <c r="G4" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>

</xml_diff>

<commit_message>
fix population to concentration conversion mathematics; fix and add multiple ODE (deterministic, semantic) test cases; these cases verify:, 00001, 00002, 00003, 00004, 00005, 00006, 00010, 00014, 00017, 00018, 00019, 00020, 00022, 00028; but these don't: 00015, 00021
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/semantic/00001/00001-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/semantic/00001/00001-wc_lang.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
-  <workbookPr showObjects="placeholders"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/semantic/00001/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="7160" windowWidth="34180" windowHeight="5060" tabRatio="500" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="1260" yWindow="10260" windowWidth="32320" windowHeight="5020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1180" yWindow="15340" windowWidth="35880" windowHeight="6200" tabRatio="500" firstSheet="3" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4228,7 +4229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="209">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 16:22:38'</t>
   </si>
@@ -4710,15 +4711,15 @@
     <t>cellular_compartment</t>
   </si>
   <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
     <t>gram</t>
   </si>
   <si>
     <t>normal_distribution</t>
   </si>
   <si>
+    <t>l</t>
+  </si>
+  <si>
     <t>density_c</t>
   </si>
   <si>
@@ -4800,31 +4801,61 @@
     <t>molecule / mole</t>
   </si>
   <si>
-    <t>c1_units</t>
-  </si>
-  <si>
-    <t>Units factor for conv_1 function for rate law 1</t>
-  </si>
-  <si>
-    <t>1 / (molecule liter)</t>
-  </si>
-  <si>
     <t>vol_c</t>
   </si>
   <si>
     <t>Volume of compartment c</t>
   </si>
   <si>
-    <t>c / density_c</t>
-  </si>
-  <si>
     <t>liter</t>
   </si>
   <si>
-    <t>test_case_00001_converted</t>
-  </si>
-  <si>
-    <t>c1_units * k1 * S1[c] * c / density_c</t>
+    <t>pop_2_conc</t>
+  </si>
+  <si>
+    <t>Convert population to concentration</t>
+  </si>
+  <si>
+    <t>1 / (Avogadro * vol_c)</t>
+  </si>
+  <si>
+    <t>mole / (molecule liter)</t>
+  </si>
+  <si>
+    <t>1 / mole</t>
+  </si>
+  <si>
+    <t>abstract_compartment</t>
+  </si>
+  <si>
+    <t>Same as specified in moles, as vol_c = 1 liter</t>
+  </si>
+  <si>
+    <t>k1 * S1[c] * pop_2_conc * vol_c * conv</t>
+  </si>
+  <si>
+    <t>conv</t>
+  </si>
+  <si>
+    <t>Conversion for rate law</t>
+  </si>
+  <si>
+    <t>Must equal volume of c in Compartments</t>
+  </si>
+  <si>
+    <t>Unit conversion for conv</t>
+  </si>
+  <si>
+    <t>1 / molecule</t>
+  </si>
+  <si>
+    <t>one_per_molecule</t>
+  </si>
+  <si>
+    <t>Avogadro * one_per_molecule</t>
+  </si>
+  <si>
+    <t>test_case_00001_pop_mass_independent</t>
   </si>
 </sst>
 </file>
@@ -4882,11 +4913,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4920,7 +4952,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -4952,11 +4984,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDA9694"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDA9694"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDA9694"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDA9694"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4980,8 +5031,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -5022,13 +5073,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5044,27 +5088,57 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5366,7 +5440,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5651,7 +5729,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5840,17 +5923,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
@@ -5905,10 +5991,10 @@
       <c r="B3" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>196</v>
       </c>
       <c r="E3" s="3"/>
@@ -5918,12 +6004,20 @@
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="33"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -5996,25 +6090,27 @@
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:I2"/>
   <dataValidations count="9">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A10">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A7:A10">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B10">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B7:B10">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C3:C10"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D3:D10"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E3:E10"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F3:F10"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G3:G10"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H3:H10">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="C7:C10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="D7:D10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="E7:E10"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="F7:F10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="G7:G10"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="H7:H10">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I3:I10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="I7:I10"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6025,7 +6121,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6058,13 +6159,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="42" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6351,11 +6452,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
@@ -6433,7 +6539,7 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>183</v>
@@ -6534,31 +6640,32 @@
   </sheetData>
   <autoFilter ref="A2:L2"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B9">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B5:B9">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A9">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A5:A9">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D3:D9">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D5:D9">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E3:E9">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E5:E9">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F3:F9"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G3:G9">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F5:F9"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;1 / second&quot; or blank." sqref="G5:G9">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H9"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I9"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J9"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K9">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H5:H9"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I5:I9"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J5:J9"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K5:K9">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L9"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L5:L9"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -6567,7 +6674,7 @@
           <x14:formula1>
             <xm:f>'!!Reactions'!$A$4:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C9</xm:sqref>
+          <xm:sqref>C5:C9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6579,7 +6686,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6829,7 +6940,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7048,7 +7163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7288,18 +7407,24 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="38" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="18" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="11" width="15.6640625" customWidth="1"/>
+    <col min="7" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7309,7 +7434,7 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="19"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="19"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -7328,10 +7453,10 @@
       <c r="C2" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="23" t="s">
         <v>104</v>
       </c>
       <c r="F2" s="21" t="s">
@@ -7354,18 +7479,18 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="30">
+      <c r="B3" s="27"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="35">
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <v>0</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="28" t="s">
         <v>174</v>
       </c>
       <c r="G3" s="3"/>
@@ -7382,13 +7507,13 @@
         <v>187</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="20">
+      <c r="D4" s="36">
         <v>1</v>
       </c>
       <c r="E4" s="20">
         <v>0</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>185</v>
       </c>
       <c r="G4" s="3"/>
@@ -7398,18 +7523,18 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="32">
+      <c r="B5" s="30"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="37">
         <v>6.0221408570000002E+23</v>
       </c>
       <c r="E5" s="20">
         <v>0</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G5" s="3"/>
@@ -7425,29 +7550,41 @@
       <c r="B6" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="20">
+      <c r="C6" s="24"/>
+      <c r="D6" s="40">
         <v>1</v>
       </c>
       <c r="E6" s="20">
         <v>0</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="24" t="s">
         <v>192</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="22" t="s">
+        <v>203</v>
+      </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="23"/>
+      <c r="A7" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>204</v>
+      </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="36">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>205</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -7458,9 +7595,9 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="20"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="26"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -7471,9 +7608,9 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="26"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -7484,7 +7621,7 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="20"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -7493,58 +7630,34 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A2:K2"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A12">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A9:A10">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B9:B10">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C3:C12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C9:C10">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D4:D12">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D9:D10">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="F3:F12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G3:G12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="H3:H12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I3:I12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="J3:J12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Enter a unit or blank." sqref="F9:F10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G9:G10"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="H9:H10"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I9:I10"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="J9:J10">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K3:K12"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="D3 E4:E12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K9:K10"/>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E9:E10">
       <formula1>-1E-100</formula1>
     </dataValidation>
   </dataValidations>
@@ -7557,7 +7670,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7748,7 +7865,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7790,42 +7911,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="42" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="S2" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="T2" s="42" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8238,7 +8359,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8268,7 +8395,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8470,25 +8597,7 @@
       <c r="L13" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="12">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="B2:L2">
-      <formula1>1</formula1>
-      <formula2>63</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:L3">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Version" error="Value must be a string." promptTitle="Version" prompt="Enter a string." sqref="B4:L4"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="URL" error="Enter a valid URL_x000a__x000a_Value must be a string._x000a__x000a_Value must be less than or equal to 65535 characters." promptTitle="URL" prompt="Enter a valid URL_x000a__x000a_Enter a string._x000a__x000a_Value must be less than or equal to 65535 characters." sqref="B5:L5">
-      <formula1>65535</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B6:L6">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revision" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B7:L7">
-      <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="wc_lang version" error="Value must be a string." promptTitle="wc_lang version" prompt="Enter a string." sqref="B8:L8"/>
+  <dataValidations count="5">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Time units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;second&quot; or blank." promptTitle="Time units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;second&quot; or blank." sqref="B9:L9">
       <formula1>"second"</formula1>
     </dataValidation>
@@ -8514,7 +8623,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8658,7 +8771,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8691,10 +8808,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="42" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -8958,7 +9075,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9310,7 +9431,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9563,7 +9688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9901,7 +10030,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10046,7 +10181,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10203,7 +10344,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10383,14 +10528,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="21" width="15.6640625" customWidth="1"/>
+    <col min="1" max="21" width="15.6640625" customWidth="1"/>
     <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10427,29 +10573,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="42" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="42" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10523,35 +10669,35 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>160</v>
+      <c r="D4" s="31" t="s">
+        <v>198</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="I4" s="37">
+      <c r="I4" s="9">
         <v>1</v>
       </c>
       <c r="J4" s="3">
         <v>0</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>163</v>
@@ -10787,7 +10933,7 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C4:C13">
       <formula1>"cellular_compartment,extracellular_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D4:D13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D5:D13">
       <formula1>"fluid_compartment,membrane_compartment"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E4:E13">
@@ -10828,12 +10974,18 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Initial density" error="Value must be a value from &quot;!!Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;!!Parameters:A&quot; or blank.">
           <x14:formula1>
             <xm:f>'!!Parameters'!$A$3:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L13 L4</xm:sqref>
+          <xm:sqref>L6:L13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Initial density" error="Value must be a value from &quot;!!Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;!!Parameters:A&quot; or blank.">
+          <x14:formula1>
+            <xm:f>'!!Parameters'!$A$3:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>L4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10845,11 +10997,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="14" width="15.6640625" customWidth="1"/>
+    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10874,22 +11033,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="42" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -11175,7 +11334,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11412,11 +11576,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="1" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="32.5" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11483,7 +11654,7 @@
         <v>168</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E3" s="17">
         <v>1.4999999999999999E-4</v>
@@ -11497,7 +11668,9 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="22" t="s">
+        <v>199</v>
+      </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11509,7 +11682,7 @@
         <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="14">
         <v>0</v>
@@ -11523,7 +11696,9 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="22" t="s">
+        <v>199</v>
+      </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -11641,29 +11816,29 @@
   </sheetData>
   <autoFilter ref="A2:L2"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A3:A12 C3:C4">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." promptTitle="Id" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters._x000a__x000a_Value must be unique." sqref="A6:A12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B6:B12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D3:D12"/>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E3:E12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." sqref="D6:D12"/>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E6:E12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F3:F12">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F6:F12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G3:G12">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G6:G12">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H3:H12"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I3:I12"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J3:J12"/>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K3:K12">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H6:H12"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="I6:I12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J6:J12"/>
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 4294967295 characters." sqref="K6:K12">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L3:L12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L6:L12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11674,7 +11849,7 @@
           <x14:formula1>
             <xm:f>'!!Species'!$A$3:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C12</xm:sqref>
+          <xm:sqref>C6:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>